<commit_message>
- Added folder creation - Deleted unused files - Fixed sdf_to_pdqt.py output
</commit_message>
<xml_diff>
--- a/excel_files/ligands_sdf_output.xlsx
+++ b/excel_files/ligands_sdf_output.xlsx
@@ -17,892 +17,892 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="296">
   <si>
+    <t>Amidosulfuron</t>
+  </si>
+  <si>
+    <t>Clethodim</t>
+  </si>
+  <si>
+    <t>Clomazone</t>
+  </si>
+  <si>
+    <t>Imazamox</t>
+  </si>
+  <si>
+    <t>Prochloraz</t>
+  </si>
+  <si>
+    <t>Rescalure</t>
+  </si>
+  <si>
+    <t>Tri-allate</t>
+  </si>
+  <si>
+    <t>Sulfosulfuron</t>
+  </si>
+  <si>
+    <t>Isofetamid</t>
+  </si>
+  <si>
+    <t>Isoxaflutole</t>
+  </si>
+  <si>
+    <t>Clopyralid</t>
+  </si>
+  <si>
+    <t>Lenacil</t>
+  </si>
+  <si>
+    <t>Florpyrauxifen-benzyl</t>
+  </si>
+  <si>
+    <t>Fenpicoxamid</t>
+  </si>
+  <si>
+    <t>Pyriproxyfen</t>
+  </si>
+  <si>
+    <t>Sulfoxaflor</t>
+  </si>
+  <si>
+    <t>Quizalofop-P-ethyl</t>
+  </si>
+  <si>
+    <t>Chlormequat</t>
+  </si>
+  <si>
+    <t>Prosulfuron</t>
+  </si>
+  <si>
+    <t>Zoxamide</t>
+  </si>
+  <si>
+    <t>(Z)-11-Hexadecenal</t>
+  </si>
+  <si>
     <t>Mandestrobin</t>
   </si>
   <si>
+    <t>2-Phenylphenol</t>
+  </si>
+  <si>
+    <t>MCPB</t>
+  </si>
+  <si>
+    <t>S-Metolachlor</t>
+  </si>
+  <si>
+    <t>1-Naphthylacetamide</t>
+  </si>
+  <si>
+    <t>Mecoprop-P</t>
+  </si>
+  <si>
+    <t>MCPA</t>
+  </si>
+  <si>
+    <t>Metazachlor</t>
+  </si>
+  <si>
+    <t>Triticonazole</t>
+  </si>
+  <si>
+    <t>Chlorotoluron</t>
+  </si>
+  <si>
+    <t>Metamitron</t>
+  </si>
+  <si>
+    <t>Captan</t>
+  </si>
+  <si>
+    <t>lambda-Cyhalothrin</t>
+  </si>
+  <si>
+    <t>Propoxycarbazone</t>
+  </si>
+  <si>
+    <t>Triclopyr</t>
+  </si>
+  <si>
+    <t>Tembotrione</t>
+  </si>
+  <si>
+    <t>Clodinafop</t>
+  </si>
+  <si>
+    <t>Benfluralin</t>
+  </si>
+  <si>
+    <t>Thifensulfuron-methyl</t>
+  </si>
+  <si>
+    <t>Dimethomorph</t>
+  </si>
+  <si>
+    <t>Ethephon</t>
+  </si>
+  <si>
+    <t>Ethylene</t>
+  </si>
+  <si>
+    <t>Propamocarb</t>
+  </si>
+  <si>
+    <t>Mepiquat</t>
+  </si>
+  <si>
+    <t>Bentazone</t>
+  </si>
+  <si>
+    <t>Hymexazol</t>
+  </si>
+  <si>
+    <t>Penconazole</t>
+  </si>
+  <si>
+    <t>Fluquinconazole</t>
+  </si>
+  <si>
+    <t>Penflufen</t>
+  </si>
+  <si>
+    <t>Flutianil</t>
+  </si>
+  <si>
+    <t>Picloram</t>
+  </si>
+  <si>
+    <t>Iodosulfuron</t>
+  </si>
+  <si>
+    <t>Bupirimate</t>
+  </si>
+  <si>
+    <t>Sedaxane</t>
+  </si>
+  <si>
+    <t>Isoxaben</t>
+  </si>
+  <si>
+    <t>Metalaxyl-M</t>
+  </si>
+  <si>
+    <t>Metconazole</t>
+  </si>
+  <si>
+    <t>Napropamide</t>
+  </si>
+  <si>
+    <t>Phosphane</t>
+  </si>
+  <si>
+    <t>Spiromesifen</t>
+  </si>
+  <si>
+    <t>(Z)-11-Hexadecen-1-ol</t>
+  </si>
+  <si>
+    <t>Formetanate</t>
+  </si>
+  <si>
+    <t>Ipconazole</t>
+  </si>
+  <si>
+    <t>Metribuzin</t>
+  </si>
+  <si>
+    <t>Trinexapac</t>
+  </si>
+  <si>
+    <t>Carvone</t>
+  </si>
+  <si>
+    <t>Malathion</t>
+  </si>
+  <si>
+    <t>Glyphosate</t>
+  </si>
+  <si>
+    <t>Bifenox</t>
+  </si>
+  <si>
+    <t>Tebuconazole</t>
+  </si>
+  <si>
+    <t>Fluometuron</t>
+  </si>
+  <si>
+    <t>Pyriofenone</t>
+  </si>
+  <si>
+    <t>Iprovalicarb</t>
+  </si>
+  <si>
+    <t>Bifenazate</t>
+  </si>
+  <si>
+    <t>Difenoconazole</t>
+  </si>
+  <si>
+    <t>Fluazinam</t>
+  </si>
+  <si>
+    <t>Chlorantraniliprole</t>
+  </si>
+  <si>
+    <t>Daminozide</t>
+  </si>
+  <si>
+    <t>Cycloxydim</t>
+  </si>
+  <si>
+    <t>Pyraclostrobin</t>
+  </si>
+  <si>
+    <t>Tetraconazole</t>
+  </si>
+  <si>
+    <t>Pinoxaden</t>
+  </si>
+  <si>
+    <t>Flazasulfuron</t>
+  </si>
+  <si>
+    <t>Mesotrione</t>
+  </si>
+  <si>
+    <t>Dimethenamid-P</t>
+  </si>
+  <si>
+    <t>24-Epibrassinolide</t>
+  </si>
+  <si>
+    <t>Cyhalofop-butyl</t>
+  </si>
+  <si>
+    <t>Pirimicarb</t>
+  </si>
+  <si>
+    <t>Pendimethalin</t>
+  </si>
+  <si>
+    <t>Valifenalate</t>
+  </si>
+  <si>
+    <t>Trifloxystrobin</t>
+  </si>
+  <si>
+    <t>Fosthiazate</t>
+  </si>
+  <si>
+    <t>Acibenzolar-S-methyl</t>
+  </si>
+  <si>
+    <t>Propaquizafop</t>
+  </si>
+  <si>
+    <t>Carfentrazone-ethyl</t>
+  </si>
+  <si>
+    <t>Prosulfocarb</t>
+  </si>
+  <si>
+    <t>Pyrimethanil</t>
+  </si>
+  <si>
+    <t>Metalaxyl</t>
+  </si>
+  <si>
+    <t>(Z)-7-Tetradecenal</t>
+  </si>
+  <si>
+    <t>Fluazifop-P</t>
+  </si>
+  <si>
+    <t>Mepanipyrim</t>
+  </si>
+  <si>
+    <t>Pyraflufen-ethyl</t>
+  </si>
+  <si>
+    <t>Metrafenone</t>
+  </si>
+  <si>
+    <t>Metam</t>
+  </si>
+  <si>
+    <t>Oxamyl</t>
+  </si>
+  <si>
+    <t>Fluxapyroxad</t>
+  </si>
+  <si>
+    <t>Indoxacarb</t>
+  </si>
+  <si>
+    <t>Fluopyram</t>
+  </si>
+  <si>
+    <t>Cyantraniliprole</t>
+  </si>
+  <si>
+    <t>Dimethachlor</t>
+  </si>
+  <si>
     <t>Penoxsulam</t>
   </si>
   <si>
-    <t>S-Metolachlor</t>
+    <t>Bixafen</t>
+  </si>
+  <si>
+    <t>Flutolanil</t>
+  </si>
+  <si>
+    <t>Gibberellins</t>
+  </si>
+  <si>
+    <t>Laminarin</t>
+  </si>
+  <si>
+    <t>Esfenvalerate</t>
+  </si>
+  <si>
+    <t>Fludioxonil</t>
+  </si>
+  <si>
+    <t>Flubendiamide</t>
+  </si>
+  <si>
+    <t>Proquinazid</t>
+  </si>
+  <si>
+    <t>Aminopyralid</t>
+  </si>
+  <si>
+    <t>Folpet</t>
+  </si>
+  <si>
+    <t>Imazalil</t>
+  </si>
+  <si>
+    <t>Metaldehyde</t>
+  </si>
+  <si>
+    <t>tau-Fluvalinate</t>
+  </si>
+  <si>
+    <t>Acrinathrin</t>
+  </si>
+  <si>
+    <t>Tritosulfuron</t>
+  </si>
+  <si>
+    <t>Flupyradifurone</t>
+  </si>
+  <si>
+    <t>Hexythiazox</t>
+  </si>
+  <si>
+    <t>Pethoxamid</t>
+  </si>
+  <si>
+    <t>(Z)-8-Tetradecen-1-ol</t>
+  </si>
+  <si>
+    <t>Foramsulfuron</t>
+  </si>
+  <si>
+    <t>1,4-Dimethylnaphthalene</t>
+  </si>
+  <si>
+    <t>Pyridaben</t>
+  </si>
+  <si>
+    <t>Propyzamide</t>
+  </si>
+  <si>
+    <t>Eugenol</t>
+  </si>
+  <si>
+    <t>Flonicamid</t>
+  </si>
+  <si>
+    <t>Fluopicolide</t>
+  </si>
+  <si>
+    <t>Thymol</t>
+  </si>
+  <si>
+    <t>Methoxyfenozide</t>
+  </si>
+  <si>
+    <t>Azoxystrobin</t>
+  </si>
+  <si>
+    <t>Diflufenican</t>
+  </si>
+  <si>
+    <t>Mesosulfuron</t>
+  </si>
+  <si>
+    <t>Isopyrazam</t>
+  </si>
+  <si>
+    <t>Ametoctradin</t>
+  </si>
+  <si>
+    <t>(E,E)-8,10-Dodecadien-1-ol</t>
+  </si>
+  <si>
+    <t>Dichlorprop-P</t>
+  </si>
+  <si>
+    <t>Flurochloridone</t>
+  </si>
+  <si>
+    <t>Fosetyl</t>
+  </si>
+  <si>
+    <t>Pirimiphos-methyl</t>
+  </si>
+  <si>
+    <t>Bromuconazole</t>
+  </si>
+  <si>
+    <t>Ethofumesate</t>
+  </si>
+  <si>
+    <t>Mandipropamid</t>
+  </si>
+  <si>
+    <t>Dodecan-1-ol</t>
+  </si>
+  <si>
+    <t>Etofenprox</t>
+  </si>
+  <si>
+    <t>Terbuthylazine</t>
+  </si>
+  <si>
+    <t>Quartz sand</t>
+  </si>
+  <si>
+    <t>Kresoxim-methyl</t>
+  </si>
+  <si>
+    <t>Fenazaquin</t>
+  </si>
+  <si>
+    <t>Phenmedipham</t>
+  </si>
+  <si>
+    <t>Sulcotrione</t>
+  </si>
+  <si>
+    <t>Triflusulfuron</t>
+  </si>
+  <si>
+    <t>Acequinocyl</t>
+  </si>
+  <si>
+    <t>Fenpropidin</t>
+  </si>
+  <si>
+    <t>Flumioxazin</t>
+  </si>
+  <si>
+    <t>Clofentezine</t>
+  </si>
+  <si>
+    <t>Bensulfuron</t>
+  </si>
+  <si>
+    <t>Oxathiapiprolin</t>
+  </si>
+  <si>
+    <t>Chromafenozide</t>
+  </si>
+  <si>
+    <t>Deltamethrin</t>
+  </si>
+  <si>
+    <t>Fenpyroximate</t>
+  </si>
+  <si>
+    <t>(Z)-9-Hexadecenal</t>
+  </si>
+  <si>
+    <t>Florasulam</t>
+  </si>
+  <si>
+    <t>Forchlorfenuron</t>
+  </si>
+  <si>
+    <t>Dithianon</t>
+  </si>
+  <si>
+    <t>Meptyldinocap</t>
+  </si>
+  <si>
+    <t>6-Benzyladenine</t>
+  </si>
+  <si>
+    <t>Metaflumizone</t>
+  </si>
+  <si>
+    <t>Quizalofop-P</t>
+  </si>
+  <si>
+    <t>Etoxazole</t>
+  </si>
+  <si>
+    <t>Geraniol</t>
+  </si>
+  <si>
+    <t>Metobromuron</t>
+  </si>
+  <si>
+    <t>Milbemectin</t>
+  </si>
+  <si>
+    <t>Flumetralin</t>
+  </si>
+  <si>
+    <t>Penthiopyrad</t>
+  </si>
+  <si>
+    <t>Cymoxanil</t>
+  </si>
+  <si>
+    <t>Dazomet</t>
+  </si>
+  <si>
+    <t>Nicosulfuron</t>
+  </si>
+  <si>
+    <t>(E)-5-Decen-1-ol</t>
+  </si>
+  <si>
+    <t>Paclobutrazol</t>
+  </si>
+  <si>
+    <t>1-methylcyclopropene</t>
+  </si>
+  <si>
+    <t>Dodemorph</t>
+  </si>
+  <si>
+    <t>Picolinafen</t>
+  </si>
+  <si>
+    <t>Tefluthrin</t>
+  </si>
+  <si>
+    <t>Halauxifen-methyl</t>
+  </si>
+  <si>
+    <t>Spirotetramat</t>
+  </si>
+  <si>
+    <t>Fluoxastrobin</t>
+  </si>
+  <si>
+    <t>Oleic_acid</t>
+  </si>
+  <si>
+    <t>Bispyribac</t>
+  </si>
+  <si>
+    <t>1-Decanol</t>
+  </si>
+  <si>
+    <t>Gamma-cyhalothrin</t>
+  </si>
+  <si>
+    <t>Cyflufenamid</t>
+  </si>
+  <si>
+    <t>Fenhexamid</t>
+  </si>
+  <si>
+    <t>Pyridalyl</t>
+  </si>
+  <si>
+    <t>Quizalofop-P-tefuryl</t>
+  </si>
+  <si>
+    <t>Cyflumetofen</t>
+  </si>
+  <si>
+    <t>Rimsulfuron</t>
+  </si>
+  <si>
+    <t>Quinmerac</t>
+  </si>
+  <si>
+    <t>Benzovindiflupyr</t>
+  </si>
+  <si>
+    <t>Tribenuron</t>
+  </si>
+  <si>
+    <t>Spiroxamine</t>
+  </si>
+  <si>
+    <t>Buprofezin</t>
+  </si>
+  <si>
+    <t>Pyridate</t>
+  </si>
+  <si>
+    <t>Benalaxyl-M</t>
+  </si>
+  <si>
+    <t>2,4-D</t>
+  </si>
+  <si>
+    <t>8-Hydroxyquinoline</t>
+  </si>
+  <si>
+    <t>Azimsulfuron</t>
+  </si>
+  <si>
+    <t>Beflubutamid</t>
+  </si>
+  <si>
+    <t>Fenoxaprop-P</t>
+  </si>
+  <si>
+    <t>Flufenacet</t>
+  </si>
+  <si>
+    <t>Fluroxypyr</t>
+  </si>
+  <si>
+    <t>Dicamba</t>
+  </si>
+  <si>
+    <t>Prohexadione</t>
+  </si>
+  <si>
+    <t>Tebufenozide</t>
+  </si>
+  <si>
+    <t>Tetradecan-1-ol</t>
+  </si>
+  <si>
+    <t>Thiencarbazone-methyl</t>
+  </si>
+  <si>
+    <t>Prothioconazole</t>
+  </si>
+  <si>
+    <t>Tolclofos-methyl</t>
+  </si>
+  <si>
+    <t>(Z)-8-Dodecen-1-ol</t>
+  </si>
+  <si>
+    <t>(Z)-13-Octadecenal</t>
+  </si>
+  <si>
+    <t>Benthiavalicarb</t>
+  </si>
+  <si>
+    <t>Pyroxsulam</t>
+  </si>
+  <si>
+    <t>Metsulfuron-methyl</t>
+  </si>
+  <si>
+    <t>Silthiofam</t>
+  </si>
+  <si>
+    <t>Mefentrifluconazole</t>
+  </si>
+  <si>
+    <t>Urea</t>
+  </si>
+  <si>
+    <t>Thiabendazole</t>
+  </si>
+  <si>
+    <t>Cyprodinil</t>
   </si>
   <si>
     <t>Halosulfuron-methyl</t>
   </si>
   <si>
-    <t>Proquinazid</t>
-  </si>
-  <si>
-    <t>Flazasulfuron</t>
-  </si>
-  <si>
-    <t>Azoxystrobin</t>
-  </si>
-  <si>
-    <t>Pyridate</t>
-  </si>
-  <si>
-    <t>Cyflumetofen</t>
+    <t>Phosmet</t>
+  </si>
+  <si>
+    <t>Cypermethrin</t>
+  </si>
+  <si>
+    <t>Cyazofamid</t>
+  </si>
+  <si>
+    <t>Diclofop</t>
+  </si>
+  <si>
+    <t>Oxyfluorfen</t>
+  </si>
+  <si>
+    <t>Amisulbrom</t>
+  </si>
+  <si>
+    <t>Dimoxystrobin</t>
   </si>
   <si>
     <t>Fenpyrazamine</t>
   </si>
   <si>
-    <t>Deltamethrin</t>
-  </si>
-  <si>
-    <t>Isopyrazam</t>
-  </si>
-  <si>
-    <t>Pyroxsulam</t>
-  </si>
-  <si>
-    <t>tau-Fluvalinate</t>
-  </si>
-  <si>
-    <t>(Z)-11-Hexadecenal</t>
-  </si>
-  <si>
-    <t>Eugenol</t>
-  </si>
-  <si>
-    <t>Quizalofop-P-ethyl</t>
-  </si>
-  <si>
-    <t>Iprovalicarb</t>
-  </si>
-  <si>
-    <t>Kresoxim-methyl</t>
-  </si>
-  <si>
-    <t>Methoxyfenozide</t>
-  </si>
-  <si>
-    <t>Acequinocyl</t>
-  </si>
-  <si>
-    <t>Gibberellins</t>
-  </si>
-  <si>
-    <t>Oxamyl</t>
-  </si>
-  <si>
-    <t>Sulcotrione</t>
-  </si>
-  <si>
-    <t>Sulfosulfuron</t>
-  </si>
-  <si>
-    <t>Prosulfocarb</t>
-  </si>
-  <si>
-    <t>Fenhexamid</t>
-  </si>
-  <si>
-    <t>Bifenox</t>
-  </si>
-  <si>
-    <t>24-Epibrassinolide</t>
-  </si>
-  <si>
-    <t>Pethoxamid</t>
-  </si>
-  <si>
-    <t>Imazamox</t>
-  </si>
-  <si>
-    <t>Zoxamide</t>
-  </si>
-  <si>
-    <t>Cymoxanil</t>
-  </si>
-  <si>
-    <t>Acibenzolar-S-methyl</t>
-  </si>
-  <si>
-    <t>Fenpropidin</t>
-  </si>
-  <si>
-    <t>Tolclofos-methyl</t>
-  </si>
-  <si>
-    <t>Ethephon</t>
-  </si>
-  <si>
-    <t>Benfluralin</t>
-  </si>
-  <si>
-    <t>Benthiavalicarb</t>
-  </si>
-  <si>
-    <t>Metconazole</t>
-  </si>
-  <si>
-    <t>Bixafen</t>
-  </si>
-  <si>
-    <t>Metobromuron</t>
-  </si>
-  <si>
-    <t>Quinmerac</t>
-  </si>
-  <si>
-    <t>Triticonazole</t>
-  </si>
-  <si>
-    <t>Florasulam</t>
-  </si>
-  <si>
-    <t>Sedaxane</t>
-  </si>
-  <si>
-    <t>(Z)-8-Dodecen-1-ol</t>
-  </si>
-  <si>
-    <t>Dazomet</t>
-  </si>
-  <si>
-    <t>Lenacil</t>
-  </si>
-  <si>
-    <t>Clethodim</t>
-  </si>
-  <si>
-    <t>Metazachlor</t>
-  </si>
-  <si>
-    <t>Mecoprop-P</t>
-  </si>
-  <si>
-    <t>Quizalofop-P-tefuryl</t>
-  </si>
-  <si>
-    <t>Formetanate</t>
-  </si>
-  <si>
-    <t>Sulfoxaflor</t>
-  </si>
-  <si>
-    <t>Flumioxazin</t>
-  </si>
-  <si>
-    <t>Tembotrione</t>
-  </si>
-  <si>
-    <t>Flutianil</t>
-  </si>
-  <si>
-    <t>(Z)-7-Tetradecenal</t>
-  </si>
-  <si>
-    <t>Foramsulfuron</t>
-  </si>
-  <si>
-    <t>Fludioxonil</t>
-  </si>
-  <si>
-    <t>6-Benzyladenine</t>
-  </si>
-  <si>
-    <t>Flutolanil</t>
-  </si>
-  <si>
-    <t>Triclopyr</t>
-  </si>
-  <si>
-    <t>Mesotrione</t>
-  </si>
-  <si>
-    <t>Benalaxyl-M</t>
-  </si>
-  <si>
-    <t>Paclobutrazol</t>
-  </si>
-  <si>
-    <t>Rescalure</t>
-  </si>
-  <si>
-    <t>Trifloxystrobin</t>
-  </si>
-  <si>
-    <t>Dimethenamid-P</t>
-  </si>
-  <si>
-    <t>1-methylcyclopropene</t>
-  </si>
-  <si>
-    <t>Tefluthrin</t>
-  </si>
-  <si>
-    <t>Chlorantraniliprole</t>
-  </si>
-  <si>
-    <t>Dodecan-1-ol</t>
-  </si>
-  <si>
-    <t>Phosmet</t>
-  </si>
-  <si>
-    <t>Amisulbrom</t>
-  </si>
-  <si>
-    <t>Azimsulfuron</t>
-  </si>
-  <si>
-    <t>Hymexazol</t>
-  </si>
-  <si>
-    <t>2-Phenylphenol</t>
-  </si>
-  <si>
-    <t>Napropamide</t>
-  </si>
-  <si>
-    <t>Esfenvalerate</t>
-  </si>
-  <si>
-    <t>Benzovindiflupyr</t>
-  </si>
-  <si>
-    <t>Chlorotoluron</t>
-  </si>
-  <si>
-    <t>MCPA</t>
-  </si>
-  <si>
-    <t>Dimethachlor</t>
-  </si>
-  <si>
-    <t>Penflufen</t>
-  </si>
-  <si>
-    <t>Pyraflufen-ethyl</t>
-  </si>
-  <si>
-    <t>Metrafenone</t>
-  </si>
-  <si>
-    <t>(Z)-8-Tetradecen-1-ol</t>
-  </si>
-  <si>
-    <t>Aminopyralid</t>
-  </si>
-  <si>
-    <t>Difenoconazole</t>
-  </si>
-  <si>
-    <t>Pirimiphos-methyl</t>
-  </si>
-  <si>
-    <t>Prohexadione</t>
-  </si>
-  <si>
-    <t>1-Decanol</t>
-  </si>
-  <si>
-    <t>Fluopyram</t>
-  </si>
-  <si>
-    <t>Isoxaben</t>
-  </si>
-  <si>
-    <t>Silthiofam</t>
-  </si>
-  <si>
-    <t>(E)-5-Decen-1-ol</t>
-  </si>
-  <si>
-    <t>Flupyradifurone</t>
-  </si>
-  <si>
-    <t>Pyridalyl</t>
-  </si>
-  <si>
-    <t>Fluazinam</t>
-  </si>
-  <si>
-    <t>Halauxifen-methyl</t>
-  </si>
-  <si>
-    <t>Flufenacet</t>
-  </si>
-  <si>
-    <t>Gamma-cyhalothrin</t>
-  </si>
-  <si>
-    <t>Amidosulfuron</t>
-  </si>
-  <si>
-    <t>lambda-Cyhalothrin</t>
-  </si>
-  <si>
-    <t>Forchlorfenuron</t>
-  </si>
-  <si>
-    <t>Metaflumizone</t>
-  </si>
-  <si>
-    <t>Penthiopyrad</t>
-  </si>
-  <si>
-    <t>Propaquizafop</t>
-  </si>
-  <si>
-    <t>Thymol</t>
-  </si>
-  <si>
-    <t>Propyzamide</t>
-  </si>
-  <si>
-    <t>Carvone</t>
-  </si>
-  <si>
-    <t>Fluroxypyr</t>
-  </si>
-  <si>
-    <t>Mefentrifluconazole</t>
-  </si>
-  <si>
-    <t>Quizalofop-P</t>
-  </si>
-  <si>
-    <t>Penconazole</t>
-  </si>
-  <si>
-    <t>Bispyribac</t>
-  </si>
-  <si>
-    <t>Prothioconazole</t>
-  </si>
-  <si>
-    <t>Cycloxydim</t>
-  </si>
-  <si>
-    <t>Prosulfuron</t>
-  </si>
-  <si>
-    <t>Pyridaben</t>
-  </si>
-  <si>
-    <t>Cyantraniliprole</t>
-  </si>
-  <si>
     <t>Tebufenpyrad</t>
   </si>
   <si>
-    <t>Laminarin</t>
-  </si>
-  <si>
-    <t>Tri-allate</t>
-  </si>
-  <si>
-    <t>Dodemorph</t>
-  </si>
-  <si>
-    <t>Metalaxyl</t>
-  </si>
-  <si>
-    <t>Tebuconazole</t>
-  </si>
-  <si>
-    <t>Cyprodinil</t>
-  </si>
-  <si>
-    <t>Metaldehyde</t>
-  </si>
-  <si>
-    <t>Pyriproxyfen</t>
-  </si>
-  <si>
-    <t>Etofenprox</t>
-  </si>
-  <si>
-    <t>Mepiquat</t>
-  </si>
-  <si>
-    <t>Fenpicoxamid</t>
-  </si>
-  <si>
-    <t>Rimsulfuron</t>
-  </si>
-  <si>
-    <t>Clopyralid</t>
-  </si>
-  <si>
-    <t>Hexythiazox</t>
-  </si>
-  <si>
-    <t>Phenmedipham</t>
-  </si>
-  <si>
-    <t>Triflusulfuron</t>
-  </si>
-  <si>
-    <t>Dicamba</t>
-  </si>
-  <si>
-    <t>Daminozide</t>
-  </si>
-  <si>
-    <t>Flumetralin</t>
-  </si>
-  <si>
-    <t>Thiencarbazone-methyl</t>
-  </si>
-  <si>
-    <t>(Z)-13-Octadecenal</t>
-  </si>
-  <si>
-    <t>Ametoctradin</t>
-  </si>
-  <si>
-    <t>Buprofezin</t>
-  </si>
-  <si>
-    <t>Terbuthylazine</t>
+    <t>Aclonifen</t>
   </si>
   <si>
     <t>Acetamiprid</t>
   </si>
   <si>
-    <t>Malathion</t>
-  </si>
-  <si>
-    <t>Pyriofenone</t>
-  </si>
-  <si>
-    <t>Cyhalofop-butyl</t>
-  </si>
-  <si>
-    <t>Mandipropamid</t>
-  </si>
-  <si>
-    <t>Metalaxyl-M</t>
-  </si>
-  <si>
-    <t>Clodinafop</t>
-  </si>
-  <si>
-    <t>Spirotetramat</t>
-  </si>
-  <si>
-    <t>2,4-D</t>
-  </si>
-  <si>
-    <t>Bupirimate</t>
-  </si>
-  <si>
-    <t>Oxathiapiprolin</t>
-  </si>
-  <si>
-    <t>Propoxycarbazone</t>
-  </si>
-  <si>
-    <t>Fluopicolide</t>
-  </si>
-  <si>
-    <t>Diclofop</t>
-  </si>
-  <si>
-    <t>Clomazone</t>
-  </si>
-  <si>
-    <t>Ipconazole</t>
-  </si>
-  <si>
-    <t>Metam</t>
-  </si>
-  <si>
-    <t>Metamitron</t>
-  </si>
-  <si>
-    <t>Pendimethalin</t>
-  </si>
-  <si>
-    <t>Fluometuron</t>
-  </si>
-  <si>
-    <t>Metsulfuron-methyl</t>
-  </si>
-  <si>
-    <t>Folpet</t>
-  </si>
-  <si>
-    <t>Oleic_acid</t>
-  </si>
-  <si>
-    <t>Carfentrazone-ethyl</t>
-  </si>
-  <si>
-    <t>MCPB</t>
-  </si>
-  <si>
-    <t>Mepanipyrim</t>
-  </si>
-  <si>
-    <t>Milbemectin</t>
-  </si>
-  <si>
-    <t>Cypermethrin</t>
-  </si>
-  <si>
-    <t>Phosphane</t>
-  </si>
-  <si>
-    <t>Pyraclostrobin</t>
-  </si>
-  <si>
-    <t>Metribuzin</t>
-  </si>
-  <si>
-    <t>Chlormequat</t>
-  </si>
-  <si>
-    <t>Fosthiazate</t>
-  </si>
-  <si>
-    <t>Flurochloridone</t>
-  </si>
-  <si>
-    <t>Bensulfuron</t>
-  </si>
-  <si>
-    <t>Nicosulfuron</t>
-  </si>
-  <si>
-    <t>Spiroxamine</t>
-  </si>
-  <si>
-    <t>1-Naphthylacetamide</t>
-  </si>
-  <si>
-    <t>Meptyldinocap</t>
-  </si>
-  <si>
-    <t>Iodosulfuron</t>
-  </si>
-  <si>
-    <t>Prochloraz</t>
-  </si>
-  <si>
-    <t>Pyrimethanil</t>
-  </si>
-  <si>
-    <t>Trinexapac</t>
-  </si>
-  <si>
-    <t>Bifenazate</t>
-  </si>
-  <si>
-    <t>Bromuconazole</t>
-  </si>
-  <si>
-    <t>Cyflufenamid</t>
-  </si>
-  <si>
-    <t>Flonicamid</t>
-  </si>
-  <si>
-    <t>Fenazaquin</t>
-  </si>
-  <si>
-    <t>Oxyfluorfen</t>
-  </si>
-  <si>
-    <t>Flubendiamide</t>
-  </si>
-  <si>
-    <t>Aclonifen</t>
-  </si>
-  <si>
-    <t>Fosetyl</t>
-  </si>
-  <si>
-    <t>Captan</t>
-  </si>
-  <si>
-    <t>Geraniol</t>
-  </si>
-  <si>
-    <t>Fluxapyroxad</t>
-  </si>
-  <si>
-    <t>Indoxacarb</t>
-  </si>
-  <si>
-    <t>Tribenuron</t>
-  </si>
-  <si>
-    <t>Picloram</t>
-  </si>
-  <si>
-    <t>Fenoxaprop-P</t>
-  </si>
-  <si>
-    <t>Bentazone</t>
-  </si>
-  <si>
-    <t>Mesosulfuron</t>
-  </si>
-  <si>
-    <t>Fluquinconazole</t>
-  </si>
-  <si>
-    <t>Thiabendazole</t>
-  </si>
-  <si>
-    <t>Tebufenozide</t>
-  </si>
-  <si>
-    <t>Urea</t>
-  </si>
-  <si>
-    <t>Valifenalate</t>
-  </si>
-  <si>
-    <t>Chromafenozide</t>
-  </si>
-  <si>
-    <t>Florpyrauxifen-benzyl</t>
-  </si>
-  <si>
-    <t>Propamocarb</t>
-  </si>
-  <si>
-    <t>Glyphosate</t>
-  </si>
-  <si>
-    <t>Ethylene</t>
-  </si>
-  <si>
-    <t>Fluazifop-P</t>
-  </si>
-  <si>
-    <t>Acrinathrin</t>
-  </si>
-  <si>
-    <t>Cyazofamid</t>
-  </si>
-  <si>
-    <t>(Z)-9-Hexadecenal</t>
-  </si>
-  <si>
-    <t>Fenpyroximate</t>
-  </si>
-  <si>
-    <t>Pirimicarb</t>
-  </si>
-  <si>
-    <t>Tetraconazole</t>
-  </si>
-  <si>
-    <t>Thifensulfuron-methyl</t>
-  </si>
-  <si>
-    <t>Tritosulfuron</t>
-  </si>
-  <si>
-    <t>Dithianon</t>
-  </si>
-  <si>
-    <t>Fluoxastrobin</t>
-  </si>
-  <si>
-    <t>Ethofumesate</t>
-  </si>
-  <si>
-    <t>Clofentezine</t>
-  </si>
-  <si>
-    <t>Tetradecan-1-ol</t>
-  </si>
-  <si>
-    <t>Imazalil</t>
-  </si>
-  <si>
-    <t>Quartz sand</t>
-  </si>
-  <si>
-    <t>Isofetamid</t>
-  </si>
-  <si>
-    <t>Isoxaflutole</t>
-  </si>
-  <si>
-    <t>Diflufenican</t>
-  </si>
-  <si>
-    <t>Beflubutamid</t>
-  </si>
-  <si>
-    <t>(Z)-11-Hexadecen-1-ol</t>
-  </si>
-  <si>
-    <t>1,4-Dimethylnaphthalene</t>
-  </si>
-  <si>
-    <t>8-Hydroxyquinoline</t>
-  </si>
-  <si>
-    <t>Etoxazole</t>
-  </si>
-  <si>
-    <t>Spiromesifen</t>
-  </si>
-  <si>
-    <t>(E,E)-8,10-Dodecadien-1-ol</t>
-  </si>
-  <si>
-    <t>Dichlorprop-P</t>
-  </si>
-  <si>
-    <t>Dimethomorph</t>
-  </si>
-  <si>
-    <t>Dimoxystrobin</t>
-  </si>
-  <si>
-    <t>Picolinafen</t>
-  </si>
-  <si>
-    <t>Pinoxaden</t>
+    <t>Sodium_4-nitrophenolate</t>
+  </si>
+  <si>
+    <t>(Z)-8-Dodecen-1-yl_acetate</t>
+  </si>
+  <si>
+    <t>(Z)-9-Tetradecen-1-yl_acetate</t>
+  </si>
+  <si>
+    <t>Potassium_bicarbonate</t>
+  </si>
+  <si>
+    <t>Dodecyl_acetate</t>
+  </si>
+  <si>
+    <t>(E,E)-7,9-Dodecadien-1-yl_acetate</t>
+  </si>
+  <si>
+    <t>(E)-11-Tetradecen-1-yl_acetate</t>
+  </si>
+  <si>
+    <t>Pelargonic_acid</t>
+  </si>
+  <si>
+    <t>(E)-8-Dodecen-1-yl_acetate</t>
+  </si>
+  <si>
+    <t>Indolylbutyric_acid</t>
+  </si>
+  <si>
+    <t>Capric_acid_(CAS_334-48-5)</t>
+  </si>
+  <si>
+    <t>Methyl_2,5-dichlorobenzoate</t>
+  </si>
+  <si>
+    <t>Gibberellic_acid</t>
+  </si>
+  <si>
+    <t>Sodium_2-nitrophenolate</t>
+  </si>
+  <si>
+    <t>Benzoic_acid</t>
+  </si>
+  <si>
+    <t>Acetic_acid</t>
+  </si>
+  <si>
+    <t>Garlic_extract</t>
+  </si>
+  <si>
+    <t>(Z,E)-Tetradeca-9,11-dienyl_acetate</t>
+  </si>
+  <si>
+    <t>Lavandulyl_senecioate</t>
+  </si>
+  <si>
+    <t>(2Z,4E)-5-[(1S)-1-Hydroxy-2,6,6-trimethyl-4-oxocyclohex-2-en-1-yl]-3-methylpenta-2,4-dienoic_acid</t>
+  </si>
+  <si>
+    <t>1-Naphthylacetic_acid</t>
+  </si>
+  <si>
+    <t>Methyl_decanoate</t>
+  </si>
+  <si>
+    <t>(Z)-9-Dodecen-1-yl_acetate</t>
+  </si>
+  <si>
+    <t>Sodium_2-methoxy-5-nitrophenolate</t>
+  </si>
+  <si>
+    <t>(Z)-11-Hexadecen-1-yl_acetate</t>
+  </si>
+  <si>
+    <t>(Z,E)-7,11-Hexadecadien-1-yl_acetate</t>
+  </si>
+  <si>
+    <t>Tetradecyl_acetate</t>
+  </si>
+  <si>
+    <t>Dodine</t>
+  </si>
+  <si>
+    <t>Boscalid_(formerly_nicobifen)</t>
+  </si>
+  <si>
+    <t>z-8-Tetradecenyl_acetate</t>
+  </si>
+  <si>
+    <t>Ziram</t>
+  </si>
+  <si>
+    <t>Caprylic_acid_(CAS_124-07-2)</t>
+  </si>
+  <si>
+    <t>(E)-5-Decen-1-yl_acetate</t>
+  </si>
+  <si>
+    <t>1-(4-Chlorophenyl)-5-(2-methoxyethoxy)-4-oxo-1,4-dihydrocinnoline-3-carboxylic_acid</t>
+  </si>
+  <si>
+    <t>Lauric_acid</t>
+  </si>
+  <si>
+    <t>Maleic_hydrazide</t>
+  </si>
+  <si>
+    <t>Orange_oil</t>
+  </si>
+  <si>
+    <t>3E,8Z-Tetradecadienyl_acetate</t>
+  </si>
+  <si>
+    <t>(Z,E)-9,12-Tetradecadien-1-yl_acetate</t>
+  </si>
+  <si>
+    <t>Sulfuryl_fluoride</t>
+  </si>
+  <si>
+    <t>(3E,8Z,11Z)-Tetradeca-3,8,11-trienyl_acetate</t>
+  </si>
+  <si>
+    <t>Methyl_octanoate</t>
+  </si>
+  <si>
+    <t>Zineb</t>
   </si>
   <si>
     <t>4-(2,4-Dichlorophenoxy)butanoic_acid</t>
   </si>
   <si>
-    <t>Caprylic_acid_(CAS_124-07-2)</t>
-  </si>
-  <si>
-    <t>Lauric_acid</t>
-  </si>
-  <si>
-    <t>Methyl_decanoate</t>
+    <t>L-Ascorbic_acid</t>
   </si>
   <si>
     <t>(Z)-11-Tetradecen-1-yl_acetate</t>
-  </si>
-  <si>
-    <t>(3E,8Z,11Z)-Tetradeca-3,8,11-trienyl_acetate</t>
-  </si>
-  <si>
-    <t>(Z)-9-Dodecen-1-yl_acetate</t>
-  </si>
-  <si>
-    <t>Dodecyl_acetate</t>
-  </si>
-  <si>
-    <t>L-Ascorbic_acid</t>
-  </si>
-  <si>
-    <t>Zineb</t>
-  </si>
-  <si>
-    <t>Dodine</t>
-  </si>
-  <si>
-    <t>Garlic_extract</t>
-  </si>
-  <si>
-    <t>Sodium_2-methoxy-5-nitrophenolate</t>
-  </si>
-  <si>
-    <t>(Z)-9-Tetradecen-1-yl_acetate</t>
-  </si>
-  <si>
-    <t>(Z,E)-9,12-Tetradecadien-1-yl_acetate</t>
-  </si>
-  <si>
-    <t>Methyl_octanoate</t>
-  </si>
-  <si>
-    <t>Sulfuryl_fluoride</t>
-  </si>
-  <si>
-    <t>Tetradecyl_acetate</t>
-  </si>
-  <si>
-    <t>Sodium_2-nitrophenolate</t>
-  </si>
-  <si>
-    <t>Ziram</t>
-  </si>
-  <si>
-    <t>(Z)-8-Dodecen-1-yl_acetate</t>
-  </si>
-  <si>
-    <t>Capric_acid_(CAS_334-48-5)</t>
-  </si>
-  <si>
-    <t>Indolylbutyric_acid</t>
-  </si>
-  <si>
-    <t>3E,8Z-Tetradecadienyl_acetate</t>
-  </si>
-  <si>
-    <t>Benzoic_acid</t>
-  </si>
-  <si>
-    <t>(Z)-11-Hexadecen-1-yl_acetate</t>
-  </si>
-  <si>
-    <t>(E)-11-Tetradecen-1-yl_acetate</t>
-  </si>
-  <si>
-    <t>Sodium_4-nitrophenolate</t>
-  </si>
-  <si>
-    <t>Potassium_bicarbonate</t>
-  </si>
-  <si>
-    <t>(E)-5-Decen-1-yl_acetate</t>
-  </si>
-  <si>
-    <t>Methyl_2,5-dichlorobenzoate</t>
-  </si>
-  <si>
-    <t>(E)-8-Dodecen-1-yl_acetate</t>
-  </si>
-  <si>
-    <t>(Z,E)-Tetradeca-9,11-dienyl_acetate</t>
-  </si>
-  <si>
-    <t>Maleic_hydrazide</t>
-  </si>
-  <si>
-    <t>Orange_oil</t>
-  </si>
-  <si>
-    <t>Pelargonic_acid</t>
-  </si>
-  <si>
-    <t>Gibberellic_acid</t>
-  </si>
-  <si>
-    <t>(2Z,4E)-5-[(1S)-1-Hydroxy-2,6,6-trimethyl-4-oxocyclohex-2-en-1-yl]-3-methylpenta-2,4-dienoic_acid</t>
-  </si>
-  <si>
-    <t>1-Naphthylacetic_acid</t>
-  </si>
-  <si>
-    <t>Acetic_acid</t>
-  </si>
-  <si>
-    <t>Boscalid_(formerly_nicobifen)</t>
-  </si>
-  <si>
-    <t>Lavandulyl_senecioate</t>
-  </si>
-  <si>
-    <t>(E,E)-7,9-Dodecadien-1-yl_acetate</t>
-  </si>
-  <si>
-    <t>(Z,E)-7,11-Hexadecadien-1-yl_acetate</t>
-  </si>
-  <si>
-    <t>1-(4-Chlorophenyl)-5-(2-methoxyethoxy)-4-oxo-1,4-dihydrocinnoline-3-carboxylic_acid</t>
-  </si>
-  <si>
-    <t>z-8-Tetradecenyl_acetate</t>
   </si>
 </sst>
 </file>

</xml_diff>